<commit_message>
AXA ROW rates update
</commit_message>
<xml_diff>
--- a/Inputs/AXA/benefits.xlsx
+++ b/Inputs/AXA/benefits.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,8 +19,199 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="E32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with OP benefit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with OP benefit
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with OP benefit
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with OP benefits
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with OP benefits
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with OP benefits
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with OP benefits
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="118">
   <si>
     <t xml:space="preserve">User Type</t>
   </si>
@@ -53,16 +243,16 @@
     <t xml:space="preserve">Annual Limit</t>
   </si>
   <si>
-    <t xml:space="preserve">USD 8,000,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD 3,200,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD 2,400,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD 1,600,000</t>
+    <t xml:space="preserve">GBP 5,000,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBP 2,000,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBP 1,500,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBP 1,000,000</t>
   </si>
   <si>
     <t xml:space="preserve">Geographical Coverage</t>
@@ -101,10 +291,10 @@
     <t xml:space="preserve">Covered in full (IP treatment restricted to 120 days per admission)</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered within OP limit of USD 9,200 (IP treatment restricted to 120 days per admission)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered within OP limit of USD 5,600 (IP treatment restricted to 120 days per admission)</t>
+    <t xml:space="preserve">Covered within OP limit of GBP 5,750 (IP treatment restricted to 120 days per admission)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered within OP limit of GBP 3,500 (IP treatment restricted to 120 days per admission)</t>
   </si>
   <si>
     <t xml:space="preserve">Not Available</t>
@@ -154,14 +344,15 @@
     <t xml:space="preserve">Covered in full </t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full within OP limit of USD 9,200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered in full within OP limit of USD 5,600
-(Optional enhanced OP cover available)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional Benefits Available</t>
+    <t xml:space="preserve">Covered in full within OP limit of GBP 5,750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default-Covered in full within OP limit of GBP 3,500
+(Optional Benefit Available)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default- Not Available
+(Optional Benefits Available)</t>
   </si>
   <si>
     <t xml:space="preserve">Out-patient Specialists/Out-patient Medicines/Vaccination/Scans &amp; Diagnostic Tests/Physiotherapy/Wellness &amp; Health Screening/Alternative Medicines/Mental Health Benefit</t>
@@ -170,10 +361,7 @@
     <t xml:space="preserve">Out-patient Specialists</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full within OP limit of USD 9,200  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered in full within OP limit of USD 5,600</t>
+    <t xml:space="preserve">Covered in full within OP limit of GBP 5,750  </t>
   </si>
   <si>
     <t xml:space="preserve">Out-patient Consultations/Out-patient Medicines/Vaccination/Scans &amp; Diagnostic Tests/Physiotherapy/Wellness &amp; Health Screening/Alternative Medicines/Mental Health Benefit</t>
@@ -182,10 +370,11 @@
     <t xml:space="preserve">Out-patient Medicines</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered up to USD 1,200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered up to USD 800</t>
+    <t xml:space="preserve">Covered up to GBP 750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default- Covered up to GBP 500
+(Optional Benefit Available)</t>
   </si>
   <si>
     <t xml:space="preserve">Out-patient Consultations/Out-patient Specialists/Vaccination/Scans &amp; Diagnostic Tests/Physiotherapy/Wellness &amp; Health Screening/Alternative Medicines/Mental Health Benefit</t>
@@ -194,13 +383,14 @@
     <t xml:space="preserve">Vaccination</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered up to USD 800 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered up to USD 480  within OP limit of USD 9,200 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered up to USD 480</t>
+    <t xml:space="preserve">Covered up to GBP 500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered up to GBP 300  within OP limit of GBP 5,750 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default- Covered up to GBP 300
+(Optional Benefit Available)</t>
   </si>
   <si>
     <t xml:space="preserve">Out-patient Consultations/Out-patient Specialists/Out-patient Medicines/Scans &amp; Diagnostic Tests/Physiotherapy/Wellness &amp; Health Screening/Alternative Medicines/Mental Health Benefit</t>
@@ -210,11 +400,12 @@
   </si>
   <si>
     <t xml:space="preserve">CT, MRI or PET scans- Covered in full 
-Diagnostic tests- Covered in full within OP limit of USD 9,200 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT, MRI or PET scans- Covered in full
-Diagnostic tests- Covered in full within OP limit of USD 5,600</t>
+Diagnostic tests- Covered in full within OP limit of GBP 5,750 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default- CT, MRI or PET scans- Covered in full
+Diagnostic tests- Covered in full within OP limit of GBP 3,500
+(Optional Benefit Available)</t>
   </si>
   <si>
     <t xml:space="preserve">Out-patient Consultations/Out-patient Specialists/Out-patient Medicines/Vaccination/Physiotherapy/Wellness &amp; Health Screening/Alternative Medicines/Mental Health Benefit</t>
@@ -226,6 +417,10 @@
     <t xml:space="preserve">Covered in full up to a maximum of 35 sessions </t>
   </si>
   <si>
+    <t xml:space="preserve">Default- Covered in full within OP limit of GBP 3,500
+(Optional Benefit Available)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Out-patient Consultations/Out-patient Specialists/Out-patient Medicines/Vaccination/Scans &amp; Diagnostic Tests/Wellness &amp; Health Screening/Alternative Medicines/Mental Health Benefit</t>
   </si>
   <si>
@@ -235,10 +430,10 @@
     <t xml:space="preserve">Maternity (Consultations, Scans and Delivery)</t>
   </si>
   <si>
-    <t xml:space="preserve">OP and IP covered up to USD 19,000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OP and IP covered up to USD 16,000 </t>
+    <t xml:space="preserve">OP and IP covered up to GBP 12,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OP and IP covered up to GBP 10,000 </t>
   </si>
   <si>
     <t xml:space="preserve">Maternity Waiting Period</t>
@@ -262,19 +457,19 @@
     <t xml:space="preserve">Dental</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered up to USD 5,600 with 20% co-pay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered up to USD 800 with 50% co-pay
+    <t xml:space="preserve">Covered up to GBP 3,500 with 20% co-pay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default- Covered up to GBP 500 with 50% co-pay
 (Optional Benefit Available)</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered up to USD 510 with 50% co-pay
-(Optional benefit available)
+    <t xml:space="preserve">Covered up to GBP 320 with 50% co-pay
+(Optional Benefit Available)
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Covered up to USD 510 with 50% co-pay
+    <t xml:space="preserve">Covered up to GBP 320 with 50% co-pay
 </t>
   </si>
   <si>
@@ -291,24 +486,28 @@
   </si>
   <si>
     <t xml:space="preserve">Eye test covered in full for one test a year 
-Prescription glasses and contact lenses covered up to USD 320  </t>
+Prescription glasses and contact lenses covered up to GBP 200</t>
   </si>
   <si>
     <t xml:space="preserve">Eye test covered in full for one test a year
-Prescription glasses and contact lenses covered up to USD 160  </t>
+Prescription glasses and contact lenses covered up to GBP 100  </t>
   </si>
   <si>
     <t xml:space="preserve">Eye test covered in full for one test a year
-Prescription glasses and contact lenses covered up to USD 160</t>
+Prescription glasses and contact lenses covered up to GBP 100</t>
   </si>
   <si>
     <t xml:space="preserve">Wellness &amp; Health Screening</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered up to USD 640 for one health check per year  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered up to USD 480 for one health check per year</t>
+    <t xml:space="preserve">Covered up to GBP 400 for one health check per year  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered up to GBP 300 for one health check per year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default- Not Available
+(Optional Benefit Available)</t>
   </si>
   <si>
     <t xml:space="preserve">Out-patient Consultations/Out-patient Specialists/Out-patient Medicines/Vaccination/Scans &amp; Diagnostic Tests/Physiotherapy/Alternative Medicines/Mental Health Benefit</t>
@@ -318,14 +517,15 @@
   </si>
   <si>
     <t xml:space="preserve">Complementary practitioner fees covered in full up to a maximum of 35 sessions
-Chinese herbal medicine covered up to 15 sessions at USD 160 per session  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complementary practitioner fees covered up to USD 480 within OP limit of USD 9,200 
+Chinese herbal medicine covered up to 15 sessions at GBP 100 per session  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complementary practitioner fees covered up to GBP 300 within OP limit of GBP 5,750 
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Complementary practitioner fees covered up to USD 480 within OP limit of USD 5,600
+    <t xml:space="preserve">Default- Complementary practitioner fees covered up to GBP 300 within OP limit of GBP 3,500
+(Optional Benefit Available)
 </t>
   </si>
   <si>
@@ -338,10 +538,11 @@
     <t xml:space="preserve">Psychiatric treatment covered in full  (IP treatment restricted to 100 days )</t>
   </si>
   <si>
-    <t xml:space="preserve">Psychiatric treatment covered up to USD 480 within OP limit of USD 9,200 (IP treatment restricted to 100 days )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psychiatric treatment covered within OP limit of USD 9,200 (IP treatment restricted to 100 days )</t>
+    <t xml:space="preserve">Psychiatric treatment covered up to GBP 300 within OP limit of GBP 5,750 (IP treatment restricted to 100 days )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default- Psychiatric treatment covered within OP limit of GBP 5,750 (IP treatment restricted to 100 days)
+(Optional Benefit Available)</t>
   </si>
   <si>
     <t xml:space="preserve">Out-patient Consultations/Out-patient Specialists/Out-patient Medicines/Vaccination/Scans &amp; Diagnostic Tests/Physiotherapy/Wellness &amp; Health Screening/Alternative Medicines</t>
@@ -383,7 +584,10 @@
     <t xml:space="preserve">Copays</t>
   </si>
   <si>
-    <t xml:space="preserve">‌NIL excess per annum/USD 160 excess per annum/USD 400 excess per annum/USD 800 excess per annum/USD 1,600 excess per annum/USD 3,200 excess per annum</t>
+    <t xml:space="preserve">NIL per year excess/GBP 100 per year excess/GBP 250 per year excess/GBP 500 per year excess/GBP 1,000 per year excess/GBP 2,000 per year excess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIL per year excess/GBP 100 per year excess/GBP 250 per year excess/GBP 500 per year excess/GBP 1,000 per year excess/GBP 2,000 per year excess/GBP 5,000 per year excess/GBP 10,000 per year excess</t>
   </si>
 </sst>
 </file>
@@ -393,7 +597,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -495,6 +699,33 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -557,7 +788,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -626,11 +857,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -642,24 +873,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -678,8 +909,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -761,11 +996,11 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="61.07"/>
@@ -927,7 +1162,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="90.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
         <v>23</v>
       </c>
@@ -1091,7 +1326,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" s="20" customFormat="true" ht="26.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="20" customFormat="true" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
         <v>20</v>
       </c>
@@ -1107,17 +1342,17 @@
       <c r="E16" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="18" t="s">
         <v>45</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="20" customFormat="true" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
         <v>20</v>
       </c>
@@ -1130,117 +1365,117 @@
       <c r="D17" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" s="20" customFormat="true" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="F18" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" s="20" customFormat="true" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="D19" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="E19" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="F19" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" s="20" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" s="20" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>42</v>
       </c>
       <c r="D20" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="F20" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" s="20" customFormat="true" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>65</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="17" t="s">
+      <c r="E21" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="18" t="s">
         <v>45</v>
       </c>
       <c r="H21" s="20" t="s">
@@ -1267,19 +1502,19 @@
       <c r="B23" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="6" t="s">
+      <c r="E23" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="21" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1290,19 +1525,19 @@
       <c r="B24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="21" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1313,19 +1548,19 @@
       <c r="B25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="6" t="s">
+      <c r="E25" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="21" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1336,19 +1571,19 @@
       <c r="B26" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="6" t="s">
+      <c r="C26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="21" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1365,7 +1600,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="39.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
@@ -1424,105 +1659,105 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F31" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" s="20" customFormat="true" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="21" t="s">
         <v>91</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="21" t="s">
         <v>28</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" s="20" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" s="20" customFormat="true" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="24" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="C33" s="25" t="s">
         <v>95</v>
       </c>
+      <c r="D33" s="25" t="s">
+        <v>96</v>
+      </c>
       <c r="E33" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="F33" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="17" t="s">
+      <c r="G33" s="18" t="s">
         <v>45</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" s="20" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" s="20" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="24" t="s">
         <v>20</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="C34" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="D34" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="E34" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G34" s="17" t="s">
+      <c r="G34" s="18" t="s">
         <v>45</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,22 +1765,22 @@
         <v>23</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>104</v>
+      <c r="C35" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,22 +1788,22 @@
         <v>20</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>106</v>
+      <c r="C36" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,7 +1811,7 @@
         <v>20</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -1589,22 +1824,22 @@
         <v>20</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,22 +1847,22 @@
         <v>20</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1635,7 +1870,7 @@
         <v>18</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -1648,7 +1883,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -1661,7 +1896,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -1674,7 +1909,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -1682,27 +1917,27 @@
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="45.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F44" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="G44" s="30" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="G44" s="31" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,33 +1973,11 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>